<commit_message>
Updated "Id" & changed the excel with display name
</commit_message>
<xml_diff>
--- a/jcp-v2/04-rsconnectProfiles/LOT_Div1-20Feb_v2_10Rows.xlsx
+++ b/jcp-v2/04-rsconnectProfiles/LOT_Div1-20Feb_v2_10Rows.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive-Official\OneDrive - Riversand Technologies, Inc\Official\00_Riversand\02_Projects\JCPenny\Data\Catalog_Export\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\#SrcCode\GitHub-RS\dataplatform-sampledata\jcp-v2\04-rsconnectProfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,20 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="148">
-  <si>
-    <t>Product Id</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="146">
   <si>
     <t>Creation Date</t>
   </si>
   <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
     <t>Display Name</t>
   </si>
   <si>
@@ -47,156 +38,12 @@
     <t>Online Only</t>
   </si>
   <si>
-    <t>Short Nm</t>
-  </si>
-  <si>
-    <t>Prod Sz Rng Tx</t>
-  </si>
-  <si>
-    <t>Prim Im Id</t>
-  </si>
-  <si>
-    <t>Chnl Cd</t>
-  </si>
-  <si>
-    <t>Model Id</t>
-  </si>
-  <si>
-    <t>Truk Itm In</t>
-  </si>
-  <si>
-    <t>Whse Class Cd</t>
-  </si>
-  <si>
-    <t>Drct Shp Rstr Id</t>
-  </si>
-  <si>
-    <t>Disposal Fee Id</t>
-  </si>
-  <si>
-    <t>Will Call Rstr Id</t>
-  </si>
-  <si>
-    <t>Fs Vendor Id</t>
-  </si>
-  <si>
-    <t>Questional Ord Qy</t>
-  </si>
-  <si>
-    <t>Lot Typ Cd</t>
-  </si>
-  <si>
-    <t>Stus Cd</t>
-  </si>
-  <si>
-    <t>White Gloved Dlvry In</t>
-  </si>
-  <si>
-    <t>Style Tx</t>
-  </si>
-  <si>
-    <t>Lot Seln Typ Cd</t>
-  </si>
-  <si>
-    <t>Non Contntl Prepaid Cd</t>
-  </si>
-  <si>
-    <t>Contntl Prepaid Cd</t>
-  </si>
-  <si>
-    <t>Subdiv Id</t>
-  </si>
-  <si>
-    <t>Unusual Dmd Qy</t>
-  </si>
-  <si>
-    <t>Div Id</t>
-  </si>
-  <si>
-    <t>Mlbl Itm In</t>
-  </si>
-  <si>
-    <t>Brand Id</t>
-  </si>
-  <si>
-    <t>Prod Length Nb</t>
-  </si>
-  <si>
-    <t>Prod Height Nb</t>
-  </si>
-  <si>
-    <t>Prod Wt Nb</t>
-  </si>
-  <si>
-    <t>Prod Width Nb</t>
-  </si>
-  <si>
-    <t>Cmrcl Carr Cd</t>
-  </si>
-  <si>
     <t>Non Cmrcl Carr Cd</t>
   </si>
   <si>
-    <t>Sabrix Commodity Cd</t>
-  </si>
-  <si>
-    <t>Pgm Typ Cd</t>
-  </si>
-  <si>
-    <t>Spcl In</t>
-  </si>
-  <si>
-    <t>Warr Id</t>
-  </si>
-  <si>
-    <t>Srvc Factsheet Id</t>
-  </si>
-  <si>
-    <t>Paranthetic Am</t>
-  </si>
-  <si>
-    <t>Will Call Fs In</t>
-  </si>
-  <si>
-    <t>Intl Shippable In</t>
-  </si>
-  <si>
-    <t>Mfr Nm</t>
-  </si>
-  <si>
-    <t>Orig Cntry Cd</t>
-  </si>
-  <si>
-    <t>Sz Unit Tx</t>
-  </si>
-  <si>
-    <t>Wt Unit Tx</t>
-  </si>
-  <si>
-    <t>Sephora In</t>
-  </si>
-  <si>
-    <t>Is Recyclable In</t>
-  </si>
-  <si>
-    <t>Model Nb</t>
-  </si>
-  <si>
     <t>Frn In</t>
   </si>
   <si>
-    <t>Child Sku</t>
-  </si>
-  <si>
-    <t>Product Attributes</t>
-  </si>
-  <si>
-    <t>Lot Alt Images</t>
-  </si>
-  <si>
-    <t>Parent Pdp</t>
-  </si>
-  <si>
     <t>1071108</t>
   </si>
   <si>
@@ -468,19 +315,172 @@
   </si>
   <si>
     <t>pp5004780288</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>On-Site Date</t>
+  </si>
+  <si>
+    <t>Off-Site Date</t>
+  </si>
+  <si>
+    <t>Short Name</t>
+  </si>
+  <si>
+    <t>Product Type</t>
+  </si>
+  <si>
+    <t>Brand LOGO Image</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>Model Number</t>
+  </si>
+  <si>
+    <t>Truck Item</t>
+  </si>
+  <si>
+    <t>Whse Supplier 1</t>
+  </si>
+  <si>
+    <t>Direct Ship Restrict Code</t>
+  </si>
+  <si>
+    <t>Disposal Fee Code</t>
+  </si>
+  <si>
+    <t>Will Call Factory Ship</t>
+  </si>
+  <si>
+    <t>Fashion Pyramid</t>
+  </si>
+  <si>
+    <t>Questionable Order Quantity</t>
+  </si>
+  <si>
+    <t>Lot Type</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>White Gloved Delivery</t>
+  </si>
+  <si>
+    <t>Style Text</t>
+  </si>
+  <si>
+    <t>Lot Selection Type</t>
+  </si>
+  <si>
+    <t>Non Continental Transportation Prepaid</t>
+  </si>
+  <si>
+    <t>Continental Tranportation Prepaid</t>
+  </si>
+  <si>
+    <t>Sub-Divisions</t>
+  </si>
+  <si>
+    <t>Unusual Demand Quantity</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Mailable Indicator</t>
+  </si>
+  <si>
+    <t>Brand</t>
+  </si>
+  <si>
+    <t>Product Length</t>
+  </si>
+  <si>
+    <t>Product Height</t>
+  </si>
+  <si>
+    <t>Product Weight</t>
+  </si>
+  <si>
+    <t>Product Width</t>
+  </si>
+  <si>
+    <t>Special Item Code</t>
+  </si>
+  <si>
+    <t>Sabrix Commodity Code</t>
+  </si>
+  <si>
+    <t>Special Program Type</t>
+  </si>
+  <si>
+    <t>Program Type</t>
+  </si>
+  <si>
+    <t>Warranty</t>
+  </si>
+  <si>
+    <t>Factsheet</t>
+  </si>
+  <si>
+    <t>Paranthetic Amount</t>
+  </si>
+  <si>
+    <t>International Shippable</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Country Of Origin</t>
+  </si>
+  <si>
+    <t>Unit of Size</t>
+  </si>
+  <si>
+    <t>Unit of Weight</t>
+  </si>
+  <si>
+    <t>Sephora</t>
+  </si>
+  <si>
+    <t>Recycle Fee</t>
+  </si>
+  <si>
+    <t>SKU Grouping</t>
+  </si>
+  <si>
+    <t>Sub Product Type</t>
+  </si>
+  <si>
+    <t>Promotional Image</t>
+  </si>
+  <si>
+    <t>Product Review Quote Text</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -503,9 +503,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -788,207 +791,212 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>97</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" t="s">
+        <v>105</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="S1" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" t="s">
+        <v>112</v>
+      </c>
+      <c r="U1" t="s">
+        <v>113</v>
+      </c>
+      <c r="V1" t="s">
+        <v>114</v>
+      </c>
+      <c r="W1" t="s">
+        <v>115</v>
+      </c>
+      <c r="X1" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>120</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="AL1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>109</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>104</v>
+      </c>
+      <c r="BA1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>43</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>44</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>45</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>46</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>50</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>51</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>52</v>
-      </c>
       <c r="BB1" t="s">
-        <v>53</v>
+        <v>142</v>
       </c>
       <c r="BC1" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
       <c r="BD1" t="s">
-        <v>55</v>
+        <v>144</v>
       </c>
       <c r="BE1" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -997,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="R2">
         <v>194027</v>
@@ -1009,7 +1017,7 @@
         <v>0</v>
       </c>
       <c r="W2" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="X2">
         <v>1</v>
@@ -1066,10 +1074,10 @@
         <v>0</v>
       </c>
       <c r="AV2" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="AW2" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="AX2">
         <v>0</v>
@@ -1078,39 +1086,39 @@
         <v>10711080018</v>
       </c>
       <c r="BC2" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="BD2" t="s">
-        <v>68</v>
+        <v>17</v>
       </c>
       <c r="BE2" t="s">
-        <v>69</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -1119,7 +1127,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="R3">
         <v>194027</v>
@@ -1131,7 +1139,7 @@
         <v>0</v>
       </c>
       <c r="W3" t="s">
-        <v>62</v>
+        <v>11</v>
       </c>
       <c r="X3">
         <v>1</v>
@@ -1188,10 +1196,10 @@
         <v>0</v>
       </c>
       <c r="AV3" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="AW3" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="AX3">
         <v>0</v>
@@ -1200,39 +1208,39 @@
         <v>10711070018</v>
       </c>
       <c r="BC3" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="BD3" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="BE3" t="s">
-        <v>74</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>75</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>76</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>77</v>
+        <v>26</v>
       </c>
       <c r="F4" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>79</v>
+        <v>28</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -1241,7 +1249,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>64</v>
+        <v>13</v>
       </c>
       <c r="R4">
         <v>194027</v>
@@ -1253,7 +1261,7 @@
         <v>0</v>
       </c>
       <c r="W4" t="s">
-        <v>78</v>
+        <v>27</v>
       </c>
       <c r="X4">
         <v>1</v>
@@ -1310,10 +1318,10 @@
         <v>0</v>
       </c>
       <c r="AV4" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="AW4" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="AX4">
         <v>0</v>
@@ -1322,36 +1330,36 @@
         <v>10711090018</v>
       </c>
       <c r="BC4" t="s">
-        <v>67</v>
+        <v>16</v>
       </c>
       <c r="BD4" t="s">
-        <v>80</v>
+        <v>29</v>
       </c>
       <c r="BE4" t="s">
-        <v>81</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D5" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="F5" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="J5" t="s">
-        <v>88</v>
+        <v>37</v>
       </c>
       <c r="K5">
         <v>2</v>
@@ -1360,7 +1368,7 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="R5">
         <v>103341</v>
@@ -1375,7 +1383,7 @@
         <v>1</v>
       </c>
       <c r="W5" t="s">
-        <v>87</v>
+        <v>36</v>
       </c>
       <c r="X5">
         <v>1</v>
@@ -1438,45 +1446,45 @@
         <v>1</v>
       </c>
       <c r="AV5" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="AW5" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="BB5" t="s">
-        <v>90</v>
+        <v>39</v>
       </c>
       <c r="BC5" t="s">
-        <v>91</v>
+        <v>40</v>
       </c>
       <c r="BD5" t="s">
-        <v>92</v>
+        <v>41</v>
       </c>
       <c r="BE5" t="s">
-        <v>93</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>94</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="E6" t="s">
-        <v>96</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="J6" t="s">
-        <v>98</v>
+        <v>47</v>
       </c>
       <c r="K6">
         <v>2</v>
@@ -1485,7 +1493,7 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="R6">
         <v>103341</v>
@@ -1500,7 +1508,7 @@
         <v>1</v>
       </c>
       <c r="W6" t="s">
-        <v>97</v>
+        <v>46</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -1563,45 +1571,45 @@
         <v>1</v>
       </c>
       <c r="AV6" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="AW6" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="BB6" t="s">
-        <v>99</v>
+        <v>48</v>
       </c>
       <c r="BC6" t="s">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="BD6" t="s">
-        <v>101</v>
+        <v>50</v>
       </c>
       <c r="BE6" t="s">
-        <v>102</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>103</v>
+        <v>52</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>105</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="J7" t="s">
-        <v>107</v>
+        <v>56</v>
       </c>
       <c r="K7">
         <v>2</v>
@@ -1610,7 +1618,7 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="R7">
         <v>103341</v>
@@ -1625,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="W7" t="s">
-        <v>106</v>
+        <v>55</v>
       </c>
       <c r="X7">
         <v>1</v>
@@ -1688,45 +1696,45 @@
         <v>1</v>
       </c>
       <c r="AV7" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="AW7" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="BB7" t="s">
-        <v>108</v>
+        <v>57</v>
       </c>
       <c r="BC7" t="s">
-        <v>109</v>
+        <v>58</v>
       </c>
       <c r="BD7" t="s">
-        <v>110</v>
+        <v>59</v>
       </c>
       <c r="BE7" t="s">
-        <v>111</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>114</v>
+        <v>63</v>
       </c>
       <c r="F8" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="J8" t="s">
-        <v>116</v>
+        <v>65</v>
       </c>
       <c r="K8">
         <v>2</v>
@@ -1735,7 +1743,7 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="R8">
         <v>103341</v>
@@ -1750,7 +1758,7 @@
         <v>1</v>
       </c>
       <c r="W8" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="X8">
         <v>1</v>
@@ -1813,45 +1821,45 @@
         <v>1</v>
       </c>
       <c r="AV8" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="AW8" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB8" t="s">
         <v>66</v>
       </c>
-      <c r="BB8" t="s">
-        <v>117</v>
-      </c>
       <c r="BC8" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="BD8" t="s">
-        <v>119</v>
+        <v>68</v>
       </c>
       <c r="BE8" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>121</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>122</v>
+        <v>71</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>123</v>
+        <v>72</v>
       </c>
       <c r="F9" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="J9" t="s">
-        <v>125</v>
+        <v>74</v>
       </c>
       <c r="K9">
         <v>2</v>
@@ -1860,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="N9" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="R9">
         <v>103341</v>
@@ -1875,7 +1883,7 @@
         <v>1</v>
       </c>
       <c r="W9" t="s">
-        <v>124</v>
+        <v>73</v>
       </c>
       <c r="X9">
         <v>1</v>
@@ -1938,45 +1946,45 @@
         <v>1</v>
       </c>
       <c r="AV9" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="AW9" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="BB9" t="s">
-        <v>126</v>
+        <v>75</v>
       </c>
       <c r="BC9" t="s">
-        <v>127</v>
+        <v>76</v>
       </c>
       <c r="BD9" t="s">
-        <v>128</v>
+        <v>77</v>
       </c>
       <c r="BE9" t="s">
-        <v>129</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>130</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>80</v>
       </c>
       <c r="C10" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>132</v>
+        <v>81</v>
       </c>
       <c r="F10" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="J10" t="s">
-        <v>134</v>
+        <v>83</v>
       </c>
       <c r="K10">
         <v>2</v>
@@ -1985,7 +1993,7 @@
         <v>0</v>
       </c>
       <c r="N10" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="R10">
         <v>103341</v>
@@ -2000,7 +2008,7 @@
         <v>1</v>
       </c>
       <c r="W10" t="s">
-        <v>133</v>
+        <v>82</v>
       </c>
       <c r="X10">
         <v>1</v>
@@ -2063,45 +2071,45 @@
         <v>1</v>
       </c>
       <c r="AV10" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="AW10" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="BB10" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="BC10" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="BD10" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
       <c r="BE10" t="s">
-        <v>138</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
       <c r="B11" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>141</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="J11" t="s">
-        <v>143</v>
+        <v>92</v>
       </c>
       <c r="K11">
         <v>2</v>
@@ -2110,7 +2118,7 @@
         <v>0</v>
       </c>
       <c r="N11" t="s">
-        <v>89</v>
+        <v>38</v>
       </c>
       <c r="R11">
         <v>103341</v>
@@ -2125,7 +2133,7 @@
         <v>1</v>
       </c>
       <c r="W11" t="s">
-        <v>142</v>
+        <v>91</v>
       </c>
       <c r="X11">
         <v>1</v>
@@ -2188,22 +2196,22 @@
         <v>1</v>
       </c>
       <c r="AV11" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="AW11" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="BB11" t="s">
-        <v>144</v>
+        <v>93</v>
       </c>
       <c r="BC11" t="s">
-        <v>145</v>
+        <v>94</v>
       </c>
       <c r="BD11" t="s">
-        <v>146</v>
+        <v>95</v>
       </c>
       <c r="BE11" t="s">
-        <v>147</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>